<commit_message>
added trip planner to gui and also resized gui
</commit_message>
<xml_diff>
--- a/src/team-seed-x-y.xlsx
+++ b/src/team-seed-x-y.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duffdl\Desktop\CSSE230\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A71578-5055-4330-A8EF-90CBA3A19576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F35A6C5-8459-4101-A637-86916D5A53E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10920" windowWidth="38620" windowHeight="21220" xr2:uid="{273045AE-3AFD-4105-B135-905FDB93D1EF}"/>
   </bookViews>
@@ -516,10 +516,10 @@
         <v>19</v>
       </c>
       <c r="C1" s="1">
-        <v>707</v>
+        <v>851</v>
       </c>
       <c r="D1" s="2">
-        <v>553</v>
+        <v>620</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -531,10 +531,10 @@
         <v>13</v>
       </c>
       <c r="C2" s="1">
-        <v>935</v>
+        <v>1124</v>
       </c>
       <c r="D2" s="1">
-        <v>340</v>
+        <v>373</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -546,10 +546,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="1">
-        <v>915</v>
+        <v>1100</v>
       </c>
       <c r="D3" s="1">
-        <v>388</v>
+        <v>429</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -561,10 +561,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="1">
-        <v>765</v>
+        <v>918</v>
       </c>
       <c r="D4" s="1">
-        <v>528</v>
+        <v>591</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -576,10 +576,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>650</v>
+        <v>778</v>
       </c>
       <c r="D5" s="1">
-        <v>365</v>
+        <v>399</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -591,10 +591,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>738</v>
+        <v>884</v>
       </c>
       <c r="D6" s="1">
-        <v>385</v>
+        <v>428</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -606,10 +606,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>488</v>
+        <v>585</v>
       </c>
       <c r="D7" s="1">
-        <v>579</v>
+        <v>655</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -621,10 +621,10 @@
         <v>12</v>
       </c>
       <c r="C8" s="1">
-        <v>360</v>
+        <v>431</v>
       </c>
       <c r="D8" s="1">
-        <v>415</v>
+        <v>458</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -636,10 +636,10 @@
         <v>29</v>
       </c>
       <c r="C9" s="1">
-        <v>720</v>
+        <v>865</v>
       </c>
       <c r="D9" s="1">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -651,10 +651,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="1">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1">
-        <v>466</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,10 +665,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="1">
-        <v>520</v>
+        <v>624</v>
       </c>
       <c r="D11" s="1">
-        <v>646</v>
+        <v>729</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -679,10 +679,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="1">
-        <v>673</v>
+        <v>809</v>
       </c>
       <c r="D12" s="1">
-        <v>417</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -693,10 +693,10 @@
         <v>16</v>
       </c>
       <c r="C13" s="1">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="D13" s="1">
-        <v>580</v>
+        <v>652</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -707,10 +707,10 @@
         <v>18</v>
       </c>
       <c r="C14" s="1">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="D14" s="1">
-        <v>534</v>
+        <v>598</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -721,10 +721,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="1">
-        <v>608</v>
+        <v>730</v>
       </c>
       <c r="D15" s="1">
-        <v>523</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,10 +735,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>777</v>
+        <v>933</v>
       </c>
       <c r="D16" s="1">
-        <v>706</v>
+        <v>804</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,10 +749,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="1">
-        <v>631</v>
+        <v>757</v>
       </c>
       <c r="D17" s="1">
-        <v>297</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -763,10 +763,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="1">
-        <v>548</v>
+        <v>658</v>
       </c>
       <c r="D18" s="1">
-        <v>276</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,10 +777,10 @@
         <v>20</v>
       </c>
       <c r="C19" s="1">
-        <v>602</v>
+        <v>720</v>
       </c>
       <c r="D19" s="1">
-        <v>651</v>
+        <v>735</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,10 +791,10 @@
         <v>23</v>
       </c>
       <c r="C20" s="1">
-        <v>871</v>
+        <v>1046</v>
       </c>
       <c r="D20" s="1">
-        <v>372</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -805,10 +805,10 @@
         <v>28</v>
       </c>
       <c r="C21" s="1">
-        <v>484</v>
+        <v>579</v>
       </c>
       <c r="D21" s="1">
-        <v>529</v>
+        <v>588</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,10 +819,10 @@
         <v>27</v>
       </c>
       <c r="C22" s="1">
-        <v>745</v>
+        <v>896</v>
       </c>
       <c r="D22" s="1">
-        <v>663</v>
+        <v>748</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,10 +833,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="1">
-        <v>864</v>
+        <v>1038</v>
       </c>
       <c r="D23" s="1">
-        <v>427</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,10 +847,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="1">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="D24" s="1">
-        <v>555</v>
+        <v>622</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,10 +861,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="1">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D25" s="1">
-        <v>254</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,10 +875,10 @@
         <v>26</v>
       </c>
       <c r="C26" s="1">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D26" s="1">
-        <v>410</v>
+        <v>453</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,10 +889,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="1">
-        <v>457</v>
+        <v>547</v>
       </c>
       <c r="D27" s="1">
-        <v>653</v>
+        <v>738</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,10 +903,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="1">
-        <v>787</v>
+        <v>942</v>
       </c>
       <c r="D28" s="1">
-        <v>305</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -917,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>229</v>
+        <v>275</v>
       </c>
       <c r="D29" s="1">
-        <v>400</v>
+        <v>441</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,10 +931,10 @@
         <v>21</v>
       </c>
       <c r="C30" s="1">
-        <v>816</v>
+        <v>978</v>
       </c>
       <c r="D30" s="1">
-        <v>450</v>
+        <v>496</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,10 +945,10 @@
         <v>31</v>
       </c>
       <c r="C31" s="1">
-        <v>526</v>
+        <v>635</v>
       </c>
       <c r="D31" s="1">
-        <v>426</v>
+        <v>469</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -959,10 +959,10 @@
         <v>34</v>
       </c>
       <c r="C32" s="1">
-        <v>328</v>
+        <v>392</v>
       </c>
       <c r="D32" s="1">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,10 +973,10 @@
         <v>33</v>
       </c>
       <c r="C33" s="1">
-        <v>569</v>
+        <v>680</v>
       </c>
       <c r="D33" s="1">
-        <v>350</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,10 +987,10 @@
         <v>32</v>
       </c>
       <c r="C34" s="1">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="D34" s="1">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>